<commit_message>
TMT0072153_TMT0072155_VerifyBanker_PrimaryOrNonPrimary_WhoIsPartOfTheActivityCanEditTheActivity - 2nd Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyBanker_PrimaryOrNonPrimary_WhoIsPartOfTheActivityCanEditTheActivity.xlsx
+++ b/TestData/TMTC0032668_VerifyBanker_PrimaryOrNonPrimary_WhoIsPartOfTheActivityCanEditTheActivity.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63DA98-BA8A-42D7-9913-6891A42C5D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C2B73-0E23-4636-AAFB-925DE5DEFAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
     <sheet name="UpdateActivity" sheetId="4" r:id="rId4"/>
+    <sheet name="MoreAttendees" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Users</t>
   </si>
@@ -550,7 +551,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,4 +733,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E65378C-1138-4771-B1D7-03B33BCC9E90}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>